<commit_message>
logt1 + cambios mi sched
</commit_message>
<xml_diff>
--- a/tspi/ciclo-1/task1/forma-task1-20105914.xlsx
+++ b/tspi/ciclo-1/task1/forma-task1-20105914.xlsx
@@ -4,13 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3480" yWindow="7760" windowWidth="29300" windowHeight="16500" tabRatio="198"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="198"/>
   </bookViews>
   <sheets>
     <sheet name="TASK" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>Tarea</t>
   </si>
@@ -92,6 +91,15 @@
   </si>
   <si>
     <t>Minuta de la reunión #1 con el cliente.</t>
+  </si>
+  <si>
+    <t>Reunión #2 con el cliente.</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>Minuta de la reunión #2 con el cliente.</t>
   </si>
 </sst>
 </file>
@@ -221,9 +229,6 @@
   </cellStyleXfs>
   <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -287,6 +292,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -618,535 +626,560 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMI21"/>
+  <dimension ref="A1:AMI20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="2"/>
-    <col min="2" max="2" width="10.83203125" style="3"/>
-    <col min="3" max="3" width="10.83203125" style="2"/>
-    <col min="4" max="6" width="10.83203125" style="3"/>
-    <col min="7" max="12" width="10.83203125" style="2"/>
-    <col min="13" max="13" width="10.83203125" style="4"/>
-    <col min="14" max="14" width="10.83203125" style="2"/>
-    <col min="15" max="16" width="10.83203125" style="5"/>
-    <col min="17" max="17" width="16.5" style="2" customWidth="1"/>
-    <col min="18" max="18" width="10.83203125" style="2"/>
-    <col min="19" max="19" width="14.5" style="2" customWidth="1"/>
-    <col min="20" max="20" width="12.1640625" style="2" customWidth="1"/>
-    <col min="21" max="1023" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="10.83203125" style="2"/>
+    <col min="3" max="3" width="10.83203125" style="1"/>
+    <col min="4" max="6" width="10.83203125" style="2"/>
+    <col min="7" max="12" width="10.83203125" style="1"/>
+    <col min="13" max="13" width="10.83203125" style="3"/>
+    <col min="14" max="14" width="10.83203125" style="1"/>
+    <col min="15" max="16" width="10.83203125" style="4"/>
+    <col min="17" max="17" width="16.5" style="1" customWidth="1"/>
+    <col min="18" max="18" width="10.83203125" style="1"/>
+    <col min="19" max="19" width="14.5" style="1" customWidth="1"/>
+    <col min="20" max="20" width="12.1640625" style="1" customWidth="1"/>
+    <col min="21" max="1023" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:20" ht="15">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1" t="s">
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1" t="s">
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="36"/>
+      <c r="Q1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
+      <c r="R1" s="36"/>
+      <c r="S1" s="36"/>
+      <c r="T1" s="36"/>
     </row>
     <row r="2" spans="1:20" ht="75">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="M2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="N2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="O2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="P2" s="10" t="s">
+      <c r="P2" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="Q2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="R2" s="6" t="s">
+      <c r="R2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="S2" s="6" t="s">
+      <c r="S2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="T2" s="7" t="s">
+      <c r="T2" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:20" s="13" customFormat="1" ht="91">
-      <c r="A3" s="14">
+    <row r="3" spans="1:20" s="12" customFormat="1" ht="91">
+      <c r="A3" s="13">
         <v>4</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="17">
+      <c r="C3" s="15"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="16">
         <v>5</v>
       </c>
-      <c r="G3" s="18">
+      <c r="G3" s="17">
         <v>2</v>
       </c>
-      <c r="H3" s="19">
+      <c r="H3" s="18">
         <v>2</v>
       </c>
-      <c r="I3" s="19">
+      <c r="I3" s="18">
         <v>2</v>
       </c>
-      <c r="J3" s="19">
+      <c r="J3" s="18">
         <v>2</v>
       </c>
-      <c r="K3" s="19">
+      <c r="K3" s="18">
         <v>2</v>
       </c>
-      <c r="L3" s="11">
+      <c r="L3" s="10">
         <f>SUM(G3:K3)</f>
         <v>10</v>
       </c>
-      <c r="M3" s="12"/>
-      <c r="N3" s="13">
+      <c r="M3" s="11"/>
+      <c r="N3" s="12">
         <v>1</v>
       </c>
-      <c r="O3" s="20">
+      <c r="O3" s="19">
         <v>41900</v>
       </c>
-      <c r="P3" s="21">
+      <c r="P3" s="20">
         <v>41900</v>
       </c>
-      <c r="Q3" s="13">
+      <c r="Q3" s="12">
         <v>2</v>
       </c>
-      <c r="R3" s="13">
+      <c r="R3" s="12">
         <v>2</v>
       </c>
-      <c r="S3" s="36">
+      <c r="S3" s="35">
         <v>41911</v>
       </c>
-      <c r="T3" s="36">
+      <c r="T3" s="35">
         <v>41911</v>
       </c>
     </row>
-    <row r="4" spans="1:20" s="13" customFormat="1" ht="52">
-      <c r="A4" s="14">
+    <row r="4" spans="1:20" s="12" customFormat="1" ht="52">
+      <c r="A4" s="13">
         <v>5</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15" t="s">
+      <c r="D4" s="14"/>
+      <c r="E4" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="17">
+      <c r="F4" s="16">
         <v>2</v>
       </c>
-      <c r="G4" s="18">
+      <c r="G4" s="17">
         <v>1</v>
       </c>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19">
+      <c r="H4" s="18"/>
+      <c r="I4" s="18">
         <v>1</v>
       </c>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="11">
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="10">
         <f>SUM(G4:K4)</f>
         <v>2</v>
       </c>
-      <c r="M4" s="12"/>
-      <c r="N4" s="13">
+      <c r="M4" s="11"/>
+      <c r="N4" s="12">
         <v>1</v>
       </c>
-      <c r="O4" s="20">
+      <c r="O4" s="19">
         <v>41901</v>
       </c>
-      <c r="P4" s="21">
+      <c r="P4" s="20">
         <v>41901</v>
       </c>
-      <c r="Q4" s="13">
+      <c r="Q4" s="12">
         <v>0.5</v>
       </c>
-      <c r="R4" s="13">
+      <c r="R4" s="12">
         <v>1</v>
       </c>
-      <c r="S4" s="36">
+      <c r="S4" s="35">
         <v>41905</v>
       </c>
-      <c r="T4" s="36">
+      <c r="T4" s="35">
         <v>41905</v>
       </c>
     </row>
-    <row r="5" spans="1:20" s="13" customFormat="1" ht="13">
-      <c r="A5" s="14"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="12"/>
-      <c r="O5" s="20"/>
-      <c r="P5" s="21"/>
-      <c r="Q5" s="22"/>
-      <c r="T5" s="23"/>
-    </row>
-    <row r="6" spans="1:20" s="13" customFormat="1" ht="13">
-      <c r="A6" s="14"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="12"/>
-      <c r="O6" s="20"/>
-      <c r="P6" s="21"/>
-      <c r="Q6" s="22"/>
-      <c r="T6" s="23"/>
-    </row>
-    <row r="7" spans="1:20" s="13" customFormat="1" ht="13">
-      <c r="A7" s="14"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="12"/>
-      <c r="O7" s="20"/>
-      <c r="P7" s="21"/>
-      <c r="Q7" s="22"/>
-      <c r="T7" s="23"/>
-    </row>
-    <row r="8" spans="1:20" s="13" customFormat="1" ht="13">
-      <c r="A8" s="14"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="11"/>
-      <c r="M8" s="12"/>
-      <c r="O8" s="20"/>
-      <c r="P8" s="21"/>
-      <c r="Q8" s="22"/>
-      <c r="T8" s="23"/>
-    </row>
-    <row r="9" spans="1:20" s="13" customFormat="1" ht="13">
-      <c r="A9" s="14"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="11"/>
-      <c r="M9" s="12"/>
-      <c r="O9" s="20"/>
-      <c r="P9" s="21"/>
-      <c r="Q9" s="22"/>
-      <c r="T9" s="23"/>
-    </row>
-    <row r="10" spans="1:20" s="13" customFormat="1" ht="13">
-      <c r="A10" s="14"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="11"/>
-      <c r="M10" s="12"/>
-      <c r="O10" s="20"/>
-      <c r="P10" s="21"/>
-      <c r="Q10" s="22"/>
-      <c r="T10" s="23"/>
-    </row>
-    <row r="11" spans="1:20" s="13" customFormat="1" ht="13">
-      <c r="A11" s="14"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19"/>
-      <c r="L11" s="11"/>
-      <c r="M11" s="12"/>
-      <c r="O11" s="20"/>
-      <c r="P11" s="21"/>
-      <c r="Q11" s="22"/>
-      <c r="T11" s="23"/>
-    </row>
-    <row r="12" spans="1:20" s="13" customFormat="1" ht="13">
-      <c r="A12" s="14"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="11"/>
-      <c r="M12" s="12"/>
-      <c r="O12" s="20"/>
-      <c r="P12" s="21"/>
-      <c r="Q12" s="22"/>
-      <c r="T12" s="23"/>
-    </row>
-    <row r="13" spans="1:20" s="13" customFormat="1" ht="13">
-      <c r="A13" s="14"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="19"/>
-      <c r="K13" s="19"/>
-      <c r="L13" s="11"/>
-      <c r="M13" s="12"/>
-      <c r="O13" s="20"/>
-      <c r="P13" s="21"/>
-      <c r="Q13" s="22"/>
-      <c r="T13" s="23"/>
-    </row>
-    <row r="14" spans="1:20" s="13" customFormat="1" ht="13">
-      <c r="A14" s="14"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="19"/>
-      <c r="K14" s="19"/>
-      <c r="L14" s="11"/>
-      <c r="M14" s="12"/>
-      <c r="O14" s="20"/>
-      <c r="P14" s="21"/>
-      <c r="Q14" s="22"/>
-      <c r="T14" s="23"/>
-    </row>
-    <row r="15" spans="1:20" s="13" customFormat="1" ht="13">
-      <c r="A15" s="14"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="19"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="19"/>
-      <c r="K15" s="19"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="12"/>
-      <c r="O15" s="20"/>
-      <c r="P15" s="21"/>
-      <c r="Q15" s="22"/>
-      <c r="T15" s="23"/>
-    </row>
-    <row r="16" spans="1:20" s="13" customFormat="1" ht="13">
-      <c r="A16" s="14"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="19"/>
-      <c r="K16" s="19"/>
-      <c r="L16" s="11"/>
-      <c r="M16" s="12"/>
-      <c r="O16" s="20"/>
-      <c r="P16" s="21"/>
-      <c r="Q16" s="22"/>
-      <c r="T16" s="23"/>
-    </row>
-    <row r="17" spans="1:20" s="13" customFormat="1" ht="13">
-      <c r="A17" s="14"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="19"/>
-      <c r="K17" s="19"/>
-      <c r="L17" s="11"/>
-      <c r="M17" s="12"/>
-      <c r="O17" s="20"/>
-      <c r="P17" s="21"/>
-      <c r="Q17" s="22"/>
-      <c r="T17" s="23"/>
-    </row>
-    <row r="18" spans="1:20" s="13" customFormat="1" ht="13">
-      <c r="A18" s="14"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="19"/>
-      <c r="K18" s="19"/>
-      <c r="L18" s="11"/>
-      <c r="M18" s="12"/>
-      <c r="O18" s="20"/>
-      <c r="P18" s="21"/>
-      <c r="Q18" s="22"/>
-      <c r="T18" s="23"/>
-    </row>
-    <row r="19" spans="1:20" s="13" customFormat="1" ht="13">
-      <c r="A19" s="14"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="19"/>
-      <c r="K19" s="19"/>
-      <c r="L19" s="11"/>
-      <c r="M19" s="12"/>
-      <c r="O19" s="20"/>
-      <c r="P19" s="21"/>
-      <c r="Q19" s="22"/>
-      <c r="T19" s="23"/>
-    </row>
-    <row r="20" spans="1:20" s="13" customFormat="1" ht="13">
-      <c r="A20" s="24"/>
-      <c r="B20" s="25"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="29"/>
-      <c r="I20" s="29"/>
-      <c r="J20" s="29"/>
-      <c r="K20" s="29"/>
-      <c r="L20" s="29"/>
-      <c r="M20" s="30"/>
-      <c r="N20" s="31"/>
-      <c r="O20" s="32"/>
-      <c r="P20" s="33"/>
-      <c r="Q20" s="34"/>
-      <c r="R20" s="31"/>
-      <c r="S20" s="31"/>
-      <c r="T20" s="35"/>
-    </row>
-    <row r="21" spans="1:20" ht="13"/>
+    <row r="5" spans="1:20" s="12" customFormat="1" ht="52">
+      <c r="A5" s="13">
+        <v>10</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="16">
+        <v>2</v>
+      </c>
+      <c r="G5" s="17"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="10">
+        <v>2</v>
+      </c>
+      <c r="M5" s="11" t="e">
+        <f t="shared" ref="M5" si="0">L5/_vtdhe</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="N5" s="12">
+        <v>1</v>
+      </c>
+      <c r="O5" s="19">
+        <v>41905</v>
+      </c>
+      <c r="P5" s="20">
+        <v>41905</v>
+      </c>
+      <c r="Q5" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="R5" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" s="12" customFormat="1">
+      <c r="A6" s="13"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="11"/>
+      <c r="O6" s="19"/>
+      <c r="P6" s="20"/>
+      <c r="Q6" s="21"/>
+      <c r="T6" s="22"/>
+    </row>
+    <row r="7" spans="1:20" s="12" customFormat="1">
+      <c r="A7" s="13"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="11"/>
+      <c r="O7" s="19"/>
+      <c r="P7" s="20"/>
+      <c r="Q7" s="21"/>
+      <c r="T7" s="22"/>
+    </row>
+    <row r="8" spans="1:20" s="12" customFormat="1">
+      <c r="A8" s="13"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="11"/>
+      <c r="O8" s="19"/>
+      <c r="P8" s="20"/>
+      <c r="Q8" s="21"/>
+      <c r="T8" s="22"/>
+    </row>
+    <row r="9" spans="1:20" s="12" customFormat="1">
+      <c r="A9" s="13"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="11"/>
+      <c r="O9" s="19"/>
+      <c r="P9" s="20"/>
+      <c r="Q9" s="21"/>
+      <c r="T9" s="22"/>
+    </row>
+    <row r="10" spans="1:20" s="12" customFormat="1">
+      <c r="A10" s="13"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="11"/>
+      <c r="O10" s="19"/>
+      <c r="P10" s="20"/>
+      <c r="Q10" s="21"/>
+      <c r="T10" s="22"/>
+    </row>
+    <row r="11" spans="1:20" s="12" customFormat="1">
+      <c r="A11" s="13"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="11"/>
+      <c r="O11" s="19"/>
+      <c r="P11" s="20"/>
+      <c r="Q11" s="21"/>
+      <c r="T11" s="22"/>
+    </row>
+    <row r="12" spans="1:20" s="12" customFormat="1">
+      <c r="A12" s="13"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="11"/>
+      <c r="O12" s="19"/>
+      <c r="P12" s="20"/>
+      <c r="Q12" s="21"/>
+      <c r="T12" s="22"/>
+    </row>
+    <row r="13" spans="1:20" s="12" customFormat="1">
+      <c r="A13" s="13"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="11"/>
+      <c r="O13" s="19"/>
+      <c r="P13" s="20"/>
+      <c r="Q13" s="21"/>
+      <c r="T13" s="22"/>
+    </row>
+    <row r="14" spans="1:20" s="12" customFormat="1">
+      <c r="A14" s="13"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="11"/>
+      <c r="O14" s="19"/>
+      <c r="P14" s="20"/>
+      <c r="Q14" s="21"/>
+      <c r="T14" s="22"/>
+    </row>
+    <row r="15" spans="1:20" s="12" customFormat="1">
+      <c r="A15" s="13"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="11"/>
+      <c r="O15" s="19"/>
+      <c r="P15" s="20"/>
+      <c r="Q15" s="21"/>
+      <c r="T15" s="22"/>
+    </row>
+    <row r="16" spans="1:20" s="12" customFormat="1">
+      <c r="A16" s="13"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="11"/>
+      <c r="O16" s="19"/>
+      <c r="P16" s="20"/>
+      <c r="Q16" s="21"/>
+      <c r="T16" s="22"/>
+    </row>
+    <row r="17" spans="1:20" s="12" customFormat="1">
+      <c r="A17" s="13"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="11"/>
+      <c r="O17" s="19"/>
+      <c r="P17" s="20"/>
+      <c r="Q17" s="21"/>
+      <c r="T17" s="22"/>
+    </row>
+    <row r="18" spans="1:20" s="12" customFormat="1">
+      <c r="A18" s="13"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="11"/>
+      <c r="O18" s="19"/>
+      <c r="P18" s="20"/>
+      <c r="Q18" s="21"/>
+      <c r="T18" s="22"/>
+    </row>
+    <row r="19" spans="1:20" s="12" customFormat="1">
+      <c r="A19" s="13"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="18"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="11"/>
+      <c r="O19" s="19"/>
+      <c r="P19" s="20"/>
+      <c r="Q19" s="21"/>
+      <c r="T19" s="22"/>
+    </row>
+    <row r="20" spans="1:20" s="12" customFormat="1">
+      <c r="A20" s="23"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="28"/>
+      <c r="J20" s="28"/>
+      <c r="K20" s="28"/>
+      <c r="L20" s="28"/>
+      <c r="M20" s="29"/>
+      <c r="N20" s="30"/>
+      <c r="O20" s="31"/>
+      <c r="P20" s="32"/>
+      <c r="Q20" s="33"/>
+      <c r="R20" s="30"/>
+      <c r="S20" s="30"/>
+      <c r="T20" s="34"/>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:F1"/>

</xml_diff>